<commit_message>
Correcting Relevance Markers Walker (2018) - Wolters (2018)
</commit_message>
<xml_diff>
--- a/simulations/cleaned_inclusion_exclusion/Walker_2018 IEC_clean/output/tables/metrics/metrics_sim.xlsx
+++ b/simulations/cleaned_inclusion_exclusion/Walker_2018 IEC_clean/output/tables/metrics/metrics_sim.xlsx
@@ -713,13 +713,13 @@
         <v>36</v>
       </c>
       <c r="C3">
-        <v>0.7244094488188977</v>
+        <v>0.7257217847769029</v>
       </c>
       <c r="D3">
-        <v>0.9041994750656168</v>
+        <v>0.9081364829396326</v>
       </c>
       <c r="E3">
-        <v>0.9816272965879265</v>
+        <v>0.9803149606299213</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -728,16 +728,16 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0.5864806201550388</v>
+        <v>0.5804237726098191</v>
       </c>
       <c r="I3">
-        <v>0.07900123000660454</v>
+        <v>0.07900748670671727</v>
       </c>
       <c r="J3">
-        <v>0.6246719160104987</v>
+        <v>0.6259842519685039</v>
       </c>
       <c r="K3">
-        <v>4142.985564304462</v>
+        <v>4143.283464566929</v>
       </c>
       <c r="L3">
         <v>76</v>
@@ -755,34 +755,34 @@
         <v>685</v>
       </c>
       <c r="Q3">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="R3">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="S3">
-        <v>1345</v>
+        <v>1371</v>
       </c>
       <c r="T3">
-        <v>4786</v>
+        <v>4885</v>
       </c>
       <c r="U3">
-        <v>10149</v>
+        <v>10425</v>
       </c>
       <c r="V3">
-        <v>47566</v>
+        <v>47577</v>
       </c>
       <c r="W3">
-        <v>47387</v>
+        <v>47388</v>
       </c>
       <c r="X3">
-        <v>46268</v>
+        <v>46242</v>
       </c>
       <c r="Y3">
-        <v>42827</v>
+        <v>42728</v>
       </c>
       <c r="Z3">
-        <v>37464</v>
+        <v>37188</v>
       </c>
       <c r="AA3">
         <v>686</v>
@@ -800,19 +800,19 @@
         <v>77</v>
       </c>
       <c r="AF3">
-        <v>0.999013</v>
+        <v>0.999244</v>
       </c>
       <c r="AG3">
-        <v>0.9952530000000001</v>
+        <v>0.995274</v>
       </c>
       <c r="AH3">
-        <v>0.971751</v>
+        <v>0.971205</v>
       </c>
       <c r="AI3">
-        <v>0.899481</v>
+        <v>0.897402</v>
       </c>
       <c r="AJ3">
-        <v>0.786844</v>
+        <v>0.781047</v>
       </c>
     </row>
   </sheetData>

</xml_diff>